<commit_message>
removed too large design for the board and started to genereta only 16 bit integer
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer16/80mhz/mxu_10x10/power.xlsx
+++ b/dtpu_configurations/only_integer16/80mhz/mxu_10x10/power.xlsx
@@ -175,19 +175,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>0.03493626043200493</v>
+        <v>0.036839623004198074</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.015047300606966019</v>
+        <v>0.016010822728276253</v>
       </c>
       <c r="D2" t="n" s="4">
-        <v>0.011129637248814106</v>
+        <v>0.011369539424777031</v>
       </c>
       <c r="E2" t="n" s="4">
-        <v>0.008358133025467396</v>
+        <v>0.008069007657468319</v>
       </c>
       <c r="F2" t="n" s="4">
-        <v>4.774295666720718E-5</v>
+        <v>6.270490848692134E-5</v>
       </c>
       <c r="G2" t="n" s="4">
         <v>0.0021374234929680824</v>
@@ -199,10 +199,10 @@
         <v>1.2604483366012573</v>
       </c>
       <c r="J2" t="n" s="4">
-        <v>0.1276429146528244</v>
+        <v>0.12766611576080322</v>
       </c>
       <c r="K2" t="n" s="4">
-        <v>1.4612503051757812</v>
+        <v>1.4641062021255493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>